<commit_message>
Mise à jour des documents pour le sprint 2
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps.xlsx
+++ b/Documents/Feuille_de_temps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AWT\NovaGo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D36C4F-6053-4423-9EC4-0FC6AEBA5846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64558C94-FB8C-4C33-80CD-B7596D466C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t>Nom</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Modèle logique</t>
+  </si>
+  <si>
+    <t>Express validator pages connexion et inscription</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -252,6 +255,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -270,7 +276,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -572,10 +578,10 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -650,7 +656,7 @@
         <v>8.5</v>
       </c>
       <c r="C5" s="6">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
@@ -744,7 +750,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
   </cols>
@@ -831,7 +837,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
   </cols>
@@ -901,10 +907,10 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -946,7 +952,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>23</v>
@@ -955,15 +961,19 @@
       <c r="H2" s="12"/>
       <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2.5</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="F3" s="12"/>
       <c r="H3" s="12"/>
       <c r="J3" s="12"/>
@@ -994,7 +1004,7 @@
       <c r="H5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -7981,7 +7991,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>

</xml_diff>

<commit_message>
Billy - feuille de sprint + feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps.xlsx
+++ b/Documents/Feuille_de_temps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2059233\GitHub\NovaGo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64558C94-FB8C-4C33-80CD-B7596D466C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B4E47F-F238-4580-A42C-1FA82C1C5DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31875" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
   <si>
     <t>Nom</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Express validator pages connexion et inscription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 </t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Diagramme de cas d'utilisation</t>
+  </si>
+  <si>
+    <t>2.5</t>
   </si>
 </sst>
 </file>
@@ -221,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -257,6 +269,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,7 +593,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -616,7 +631,7 @@
         <v>6.5</v>
       </c>
       <c r="C3" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
@@ -747,7 +762,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -794,8 +809,12 @@
       <c r="B2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -804,8 +823,12 @@
       <c r="B3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">

</xml_diff>

<commit_message>
Changement du script de creation et update de la feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps.xlsx
+++ b/Documents/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kianl\NovaGo\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76997B5F-F435-48AF-B20C-851941AC1CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AB2E20-A6B0-4A16-B394-08C6DFA81BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>Nom</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Refonte de la BD</t>
+  </si>
+  <si>
+    <t>Amélioration de la BD</t>
+  </si>
+  <si>
+    <t>Script d'insertion</t>
   </si>
 </sst>
 </file>
@@ -872,7 +878,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -925,6 +931,12 @@
       <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -938,6 +950,12 @@
       </c>
       <c r="D3" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix de la BD
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps.xlsx
+++ b/Documents/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kianl\NovaGo\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AB2E20-A6B0-4A16-B394-08C6DFA81BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59511BAE-2DC8-4093-8D7E-4DC4124D2126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3732" yWindow="696" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -878,7 +878,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -932,7 +932,7 @@
         <v>32</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Ajout de plusieurs documents
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps.xlsx
+++ b/Documents/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kianl\NovaGo\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615C216C-C027-4FD4-B4F8-01210BC71758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87424ECD-6772-4532-A147-D38E52F40A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3732" yWindow="696" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>Nom</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Script d'insertion</t>
+  </si>
+  <si>
+    <t>Faire fonctionner la BD dans docker</t>
   </si>
 </sst>
 </file>
@@ -878,7 +881,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -952,7 +955,7 @@
         <v>33</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
         <v>35</v>
@@ -967,6 +970,12 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>

</xml_diff>

<commit_message>
Derniers changements aux documents et modification exigences NF
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps.xlsx
+++ b/Documents/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165F83AE-BA41-4E36-AC1E-7D77820E92D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BC69FE-456E-45DD-B960-19356E9942F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="0" windowWidth="13800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>Nom</t>
   </si>
@@ -172,6 +172,36 @@
   </si>
   <si>
     <t>Ajout de validation avec ExpressJS</t>
+  </si>
+  <si>
+    <t>Discuter la planification</t>
+  </si>
+  <si>
+    <t>Rechercher bootstrap</t>
+  </si>
+  <si>
+    <t>principal.ejs</t>
+  </si>
+  <si>
+    <t>modifier bootstrap</t>
+  </si>
+  <si>
+    <t>Méthodologie de travail</t>
+  </si>
+  <si>
+    <t>recu-billet.ejs</t>
+  </si>
+  <si>
+    <t>Validation page d'inscription</t>
+  </si>
+  <si>
+    <t>amélioration des tableaux de cas d'utilisation</t>
+  </si>
+  <si>
+    <t>amélioration de l'apparence de la page de réservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">méthodologie de travail </t>
   </si>
 </sst>
 </file>
@@ -309,20 +339,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,9 +673,7 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -685,7 +713,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="6">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="E3" s="6">
         <v>0</v>
@@ -705,7 +733,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4" s="9">
         <v>0</v>
@@ -745,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E6" s="9">
         <v>0</v>
@@ -772,7 +800,9 @@
       <c r="C9" s="6">
         <v>5</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6">
+        <v>6</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
@@ -786,7 +816,9 @@
       <c r="C10" s="9">
         <v>6</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9">
+        <v>6</v>
+      </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
     </row>
@@ -830,15 +862,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -873,47 +907,221 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="E2" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
         <v>3.5</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15">
+        <v>1</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15">
+        <v>2</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1041,7 +1249,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1079,120 +1287,124 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="18">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="16">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="15">
         <v>1</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="15"/>
+      <c r="G2" s="15">
+        <v>1</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="18">
+      <c r="A3" s="16">
         <v>2.5</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="16">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="15">
         <v>2</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="17">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="17">
+      <c r="C4" s="16"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15">
         <v>4</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="17">
+      <c r="A5" s="15">
         <v>1</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="17">
+      <c r="C5" s="16"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15">
         <v>2</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
+      <c r="A6" s="15">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="15"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
@@ -8158,7 +8370,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8212,6 +8424,12 @@
       <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -8222,10 +8440,22 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Connexion à la BD incomplète
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps.xlsx
+++ b/Documents/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CDDAE5-82B5-4C1F-AA8A-075B0A146E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC9EF78-FA43-474C-911F-8DAD807B4BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>Nom</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Organisation d'équipe</t>
+  </si>
+  <si>
+    <t>Connexion à la BD page d'inscription</t>
   </si>
 </sst>
 </file>
@@ -677,7 +680,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -761,7 +764,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5" s="7">
         <v>0</v>
@@ -1256,7 +1259,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1341,7 +1344,7 @@
         <v>41</v>
       </c>
       <c r="G3" s="17">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>50</v>
@@ -1364,8 +1367,12 @@
       <c r="F4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="14"/>
+      <c r="G4" s="17">
+        <v>1</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="17"/>
       <c r="J4" s="14"/>
     </row>

</xml_diff>